<commit_message>
edit the site location
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/TCSA_site_locations.xlsx
+++ b/analysis/data/raw_data/TCSA_site_locations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gayoungp/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gayoungp/Desktop/tcsakoreanpaleolithic/analysis/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF6B6E3-9501-E340-8D1A-E6D5399E6A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{723322C1-5CE0-9C4D-91BF-41CB596D185B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="3260" windowWidth="28800" windowHeight="24320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26540" yWindow="2880" windowWidth="28800" windowHeight="24320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Site_info_default" sheetId="1" r:id="rId1"/>
@@ -568,7 +568,7 @@
   <dimension ref="A1:F993"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="168" zoomScaleNormal="168" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -685,10 +685,10 @@
         <v>18</v>
       </c>
       <c r="D7" s="5">
-        <v>37.56027778</v>
+        <v>37.685578</v>
       </c>
       <c r="E7" s="5">
-        <v>127.5688889</v>
+        <v>127.86057599999999</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -702,10 +702,10 @@
         <v>21</v>
       </c>
       <c r="D8" s="5">
-        <v>37.769722219999998</v>
+        <v>37.658175999999997</v>
       </c>
       <c r="E8" s="5">
-        <v>127.08750000000001</v>
+        <v>127.254599</v>
       </c>
       <c r="F8" s="6"/>
     </row>

</xml_diff>